<commit_message>
completed rough draft, take 2
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amand\OneDrive\Documents\DA14\Projects\lookups-da14-alroman14\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E89ABC-0D77-416A-BFA9-475AA67430BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8737E0-AFF2-403A-BCFF-5115A1771EFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -489,11 +489,13 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -859,7 +861,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -875,8 +877,7 @@
     <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1236,8 +1237,8 @@
   <dimension ref="A1:P102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B84" sqref="B84"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H91" sqref="H91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5170,11 +5171,6 @@
         <v>76</v>
       </c>
       <c r="B88" s="13"/>
-      <c r="C88" s="14"/>
-      <c r="D88" s="14"/>
-      <c r="E88" s="14"/>
-      <c r="F88" s="14"/>
-      <c r="G88" s="14"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
@@ -5379,7 +5375,7 @@
         <v>Metropolitan Clerk</v>
       </c>
       <c r="C99" s="12">
-        <f t="shared" ref="C99:E100" si="23">INDEX($A$2:$P$52,MATCH(B99,$A$2:$A$52,0),MATCH(_xlfn.CONCAT($A99,"_diff_pct"),$A$1:$P$1,0))</f>
+        <f t="shared" ref="C99:C100" si="23">INDEX($A$2:$P$52,MATCH(B99,$A$2:$A$52,0),MATCH(_xlfn.CONCAT($A99,"_diff_pct"),$A$1:$P$1,0))</f>
         <v>-0.17551246244575608</v>
       </c>
       <c r="D99" t="str">
@@ -5432,11 +5428,9 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="13"/>
-      <c r="B101" s="14"/>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="13"/>
-      <c r="B102" s="14"/>
     </row>
   </sheetData>
   <dataValidations count="2">

</xml_diff>